<commit_message>
NZR Shop Update 07/11/2020
</commit_message>
<xml_diff>
--- a/NZR Online Shop.xlsx
+++ b/NZR Online Shop.xlsx
@@ -852,15 +852,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0;\-#,##0"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0;\-#,##0"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="181" formatCode="[$-409]mmmm\-yy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="180" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="181" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -946,21 +946,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -975,78 +960,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1082,8 +1000,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1230,7 +1230,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,19 +1308,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1266,31 +1332,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1308,60 +1356,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1374,13 +1368,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1394,65 +1394,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1481,6 +1427,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1491,20 +1476,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1514,130 +1514,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1696,7 +1696,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1843,7 +1843,7 @@
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="8" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="8" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1852,7 +1852,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1861,7 +1861,7 @@
     <xf numFmtId="49" fontId="1" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1882,7 +1882,7 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1942,7 +1942,7 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -1962,7 +1962,7 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -1992,7 +1992,7 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -2002,7 +2002,7 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="49" formatCode="@"/>
@@ -2011,10 +2011,10 @@
       <numFmt numFmtId="49" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="49" formatCode="@"/>
@@ -8863,15 +8863,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B20 B13:B18">
       <formula1>Item!$B$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19 C20 C24 C28 C42 C48 C66 C67 C13:C18 C32:C34 C37:C38 C46:C47 C52:C56 C60:C62">
-      <formula1>"Food"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
-      <formula1>Item!$B$9:$B$14</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19:G19 I19:N19 F20:G20 I20:N20 F24:G24 I24:N24 K28:M28 K48:M48 K49:M49 K66:M66 K67:M67 K68:M68 K83:M83 K84:M84 K85:M85 K96:L96 M96 K97:M97 K71:M72 K75:M76 K79:M80 K42:M43 K46:M47 K52:M53 K88:M89 K92:M93 F13:G18 I13:N18 K37:M39 K55:M57 K32:M34 K60:M63"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19 D20 D24 D28 D42 D48 D66 D67 D71 D75 D79 D83 D84 D88 D13:D18 D32:D34 D37:D38 D46:D47 D52:D56 D60:D62">
       <formula1>$V$12:$V$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19 C20 C24 C28 C42 C48 C66 C67 C13:C18 C32:C34 C37:C38 C46:C47 C52:C56 C60:C62">
+      <formula1>"Food"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19 E20 E24 E28 E42 E48 E66 E67 E71 E75 E79 E83 E84 E88 E92 E96 E13:E18 E32:E34 E37:E38 E46:E47 E52:E56 E60:E62">
       <formula1>Supllier!$C$19:$C$25</formula1>
@@ -8884,6 +8881,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B28 B32:B34 B37:B38">
       <formula1>Item!$B$9:$B$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+      <formula1>Item!$B$9:$B$14</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48 B46:B47">
       <formula1>Item!$B$9:$B$15</formula1>
@@ -8932,8 +8932,8 @@
   <sheetPr/>
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="J90" sqref="J90"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.2857142857143" defaultRowHeight="38" customHeight="1"/>
@@ -10476,7 +10476,7 @@
       </c>
       <c r="I73" s="4">
         <f t="shared" si="3"/>
-        <v>64000</v>
+        <v>139000</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="1" customHeight="1" spans="1:9">
@@ -10494,21 +10494,21 @@
         <v>152</v>
       </c>
       <c r="E74" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F74" s="23" t="s">
         <v>172</v>
       </c>
       <c r="G74" s="4">
         <f>(C74-E74)*Pemesanan!L84</f>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>171</v>
       </c>
       <c r="I74" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="76" customFormat="1" customHeight="1" spans="1:9">
@@ -10642,21 +10642,21 @@
         <v>152</v>
       </c>
       <c r="E82" s="1">
-        <v>240</v>
+        <v>22</v>
       </c>
       <c r="F82" s="23" t="s">
         <v>172</v>
       </c>
       <c r="G82" s="4">
         <f>(C82-E82)*Pemesanan!L92</f>
-        <v>0</v>
+        <v>174400</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>171</v>
       </c>
       <c r="I82" s="4">
         <f>SUM(G82:G83)</f>
-        <v>0</v>
+        <v>174400</v>
       </c>
     </row>
     <row r="84" customFormat="1" customHeight="1" spans="1:9">
@@ -10716,21 +10716,21 @@
         <v>148</v>
       </c>
       <c r="E86" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F86" s="23" t="s">
         <v>172</v>
       </c>
       <c r="G86" s="4">
         <f>(C86-E86)*Pemesanan!L96</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>171</v>
       </c>
       <c r="I86" s="4">
         <f>SUM(G86:G87)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
@@ -10762,6 +10762,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3 A4 A5 A6 A7 A8 A9 A10">
       <formula1>Pemesanan!$F$13:$F$21</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50 A51 A52">
+      <formula1>Pemesanan!$F$60:$F$63</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4 F5 F6 F7 F8 F9 F10 F14 F18 F22 F23 F27 F28 F32 F36 F37 F38 F42 F46 F50 F51 F52 F56 F57 F61 F65 F69 F73 F74 F78 F82 F86">
       <formula1>"Available,Done"</formula1>
     </dataValidation>
@@ -10783,9 +10786,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A18">
       <formula1>Pemesanan!$F$28:$F$29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H50 H56 H57 H61 H65 H69 H73 H74 H78 H82 H86 H51:H52">
-      <formula1>"January,February,March,April,May,June,July,August,September,October,November,December"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A36 A37 A38 A42">
       <formula1>Pemesanan!$F$46:$F$49</formula1>
     </dataValidation>
@@ -10798,8 +10798,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22 A23">
       <formula1>Pemesanan!$F$32:$F$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50 A51 A52">
-      <formula1>Pemesanan!$F$60:$F$63</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H50 H56 H57 H61 H65 H69 H73 H74 H78 H82 H86 H51:H52">
+      <formula1>"January,February,March,April,May,June,July,August,September,October,November,December"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A56 A57">
       <formula1>Pemesanan!$F$66:$F$68</formula1>
@@ -12031,17 +12031,17 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
-      <formula1>"Blom dibayar,Sdh dibayar"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>Item!$B$9:$B$88</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>"Dipesan,Siap dikirim,Sdh dikirim"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>Customer!$B$3:$B$91</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>"Dipesan,Siap dikirim,Sdh dikirim"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>"Blom dibayar,Sdh dibayar"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
NZR Shop Updated 09/11/2020
</commit_message>
<xml_diff>
--- a/NZR Online Shop.xlsx
+++ b/NZR Online Shop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20925" windowHeight="9810" activeTab="3"/>
+    <workbookView windowWidth="19815" windowHeight="7830" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Supllier" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="276">
   <si>
     <t>No</t>
   </si>
@@ -842,6 +842,12 @@
   </si>
   <si>
     <t>Ibu Bina Bakti 4</t>
+  </si>
+  <si>
+    <t>Mama Nadif</t>
+  </si>
+  <si>
+    <t>Bumi Prima</t>
   </si>
   <si>
     <t>Siap dikirim</t>
@@ -855,14 +861,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="177" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="#,##0;\-#,##0"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0;\-#,##0"/>
+    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="181" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -961,16 +967,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -992,16 +990,16 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1032,15 +1030,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1069,15 +1059,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1086,6 +1077,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1232,7 +1238,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1244,73 +1328,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1322,55 +1340,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,6 +1356,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -1396,17 +1402,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1416,21 +1416,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1474,11 +1459,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1493,18 +1484,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1516,85 +1522,97 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="43" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1603,34 +1621,22 @@
     <xf numFmtId="0" fontId="11" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1639,7 +1645,7 @@
     <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1701,7 +1707,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1746,7 +1752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1758,7 +1764,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1842,7 +1848,7 @@
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="8" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1851,7 +1857,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="179" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1860,7 +1866,7 @@
     <xf numFmtId="49" fontId="1" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1881,7 +1887,7 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1941,7 +1947,7 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -1961,7 +1967,7 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -1991,7 +1997,7 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -2001,7 +2007,7 @@
         <sz val="11"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="49" formatCode="@"/>
@@ -2010,10 +2016,10 @@
       <numFmt numFmtId="49" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="49" formatCode="@"/>
@@ -6409,7 +6415,7 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
@@ -7425,7 +7431,7 @@
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
@@ -7945,10 +7951,10 @@
   <sheetPr/>
   <dimension ref="A1:AA98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="29.1" customHeight="1"/>
@@ -10354,18 +10360,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B20 B13:B18">
       <formula1>Item!$B$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52:B55">
-      <formula1>Item!$B$10:$B$17</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
-      <formula1>Item!$B$10:$B$15</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
-      <formula1>Item!$B$10:$B$21</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H48 H66 H67 H71 H75 H79 H83 H84 H88 H92 H46:H47 H52:H56 H60:H62">
-      <formula1>$Q$12:$Q$21</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19 C20 C24 C28 C42 C48 C66 C67 C13:C18 C32:C34 C37:C38 C46:C47 C52:C56 C60:C62">
       <formula1>"Food"</formula1>
     </dataValidation>
@@ -10382,8 +10376,20 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H24">
       <formula1>$Q$12:$Q$18</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52:B55">
+      <formula1>Item!$B$10:$B$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+      <formula1>Item!$B$10:$B$15</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48 B46:B47">
       <formula1>Item!$B$10:$B$16</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
+      <formula1>Item!$B$10:$B$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H48 H66 H67 H71 H75 H79 H83 H84 H88 H92 H46:H47 H52:H56 H60:H62">
+      <formula1>$Q$12:$Q$21</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
       <formula1>Item!$B$10:$B$20</formula1>
@@ -10420,7 +10426,7 @@
   <sheetPr/>
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" topLeftCell="A75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A57" workbookViewId="0">
       <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
@@ -12243,9 +12249,6 @@
     <mergeCell ref="I73:I74"/>
   </mergeCells>
   <dataValidations count="22">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4 F5 F6 F7 F8 F9 F10 F14 F18 F22 F23 F27 F28 F32 F36 F37 F38 F42 F46 F50 F51 F52 F56 F57 F61 F65 F69 F73 F74 F78 F82 F86">
-      <formula1>"Available,Done"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3 A4 A5 A6 A7 A8 A9 A10">
       <formula1>Pemesanan!$F$13:$F$21</formula1>
     </dataValidation>
@@ -12254,6 +12257,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B4 B5 B6 B7 B8 B9 B10 B14 B18 B22 B23 B27 B28 B32 B36 B37 B38 B42 B46 B50 B51 B52 B56 B57 B61 B65 B69 B73 B74 B78 B82 B86">
       <formula1>Supllier!$C$19:$C$25</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4 F5 F6 F7 F8 F9 F10 F14 F18 F22 F23 F27 F28 F32 F36 F37 F38 F42 F46 F50 F51 F52 F56 F57 F61 F65 F69 F73 F74 F78 F82 F86">
+      <formula1>"Available,Done"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A84:I84">
       <formula1>Item!$B$10:$B$46</formula1>
@@ -12426,9 +12432,9 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -13160,9 +13166,15 @@
       <c r="A49" s="10">
         <v>45</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="50" customHeight="1" spans="1:1">
       <c r="A50" s="10"/>
@@ -13360,10 +13372,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="4:6">
@@ -13529,9 +13541,6 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
-      <formula1>"Blom dibayar,Sdh dibayar"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>Item!$B$10:$B$89</formula1>
     </dataValidation>
@@ -13541,6 +13550,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
       <formula1>"Dipesan,Siap dikirim,Sdh dikirim"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>"Blom dibayar,Sdh dibayar"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>